<commit_message>
Refactor build script.  Regenerate the Excel report and Rubycritic website
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -125,9 +125,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$2:$A$13</c:f>
+              <c:f>'Chart Report'!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>xsd</c:v>
                 </c:pt>
@@ -138,30 +138,57 @@
                   <c:v>folders</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>js</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>txt</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>html</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>css</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>png</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>ttf</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>sh</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>png</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>rb</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
+                  <c:v>woff</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>eot</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>svg</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>woff2</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>md</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
+                  <c:v>exe</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>otf</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Gemfile</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>lock</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>Gemfile</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>exe</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="20">
                   <c:v>xlsx</c:v>
                 </c:pt>
               </c:strCache>
@@ -169,44 +196,71 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$2:$B$13</c:f>
+              <c:f>'Chart Report'!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>182</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>23</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="9" formatCode="General">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="12" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="17" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="18" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="19" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -276,9 +330,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$2:$A$13</c:f>
+              <c:f>'Chart Report'!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>xsd</c:v>
                 </c:pt>
@@ -289,30 +343,57 @@
                   <c:v>folders</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>js</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>txt</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>html</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>css</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>png</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>ttf</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>sh</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>png</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>rb</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
+                  <c:v>woff</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>eot</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>svg</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>woff2</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>md</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
+                  <c:v>exe</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>otf</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Gemfile</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>lock</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>Gemfile</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>exe</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="20">
                   <c:v>xlsx</c:v>
                 </c:pt>
               </c:strCache>
@@ -320,44 +401,71 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$2:$B$13</c:f>
+              <c:f>'Chart Report'!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>182</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>23</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="9" formatCode="General">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="12" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="17" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="18" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="19" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -365,11 +473,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="10832434"/>
-        <c:axId val="9688248"/>
+        <c:axId val="1182702"/>
+        <c:axId val="8456010"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="10832434"/>
+        <c:axId val="1182702"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,7 +498,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9688248"/>
+        <c:crossAx val="8456010"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -399,7 +507,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9688248"/>
+        <c:axId val="8456010"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,7 +528,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10832434"/>
+        <c:crossAx val="1182702"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -485,7 +593,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$16:$A$16</c:f>
+              <c:f>'Chart Report'!$A$25:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -496,12 +604,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$16:$B$16</c:f>
+              <c:f>'Chart Report'!$B$25:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>91</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -569,7 +677,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$19:$A$19</c:f>
+              <c:f>'Chart Report'!$A$28:$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -580,12 +688,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$19:$B$19</c:f>
+              <c:f>'Chart Report'!$B$28:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>91</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -653,7 +761,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$22:$A$23</c:f>
+              <c:f>'Chart Report'!$A$31:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -667,12 +775,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$22:$B$23</c:f>
+              <c:f>'Chart Report'!$B$31:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>84</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -743,7 +851,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$26:$A$27</c:f>
+              <c:f>'Chart Report'!$A$35:$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -757,12 +865,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$26:$B$27</c:f>
+              <c:f>'Chart Report'!$B$35:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>84</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -980,7 +1088,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1009,7 +1117,7 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>182</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
@@ -1029,13 +1137,13 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>txt</t>
+          <t>js</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
@@ -1045,192 +1153,282 @@
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>sh</t>
+          <t>txt</t>
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>png</t>
+          <t>html</t>
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>rb</t>
+          <t>css</t>
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>md</t>
+          <t>png</t>
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>lock</t>
+          <t>ttf</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>Gemfile</t>
+          <t>sh</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>exe</t>
+          <t>rb</t>
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>xlsx</t>
+          <t>woff</t>
         </is>
       </c>
       <c r="B13" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>eot</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t>Deployed Version</t>
-        </is>
-      </c>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>svg</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>2019.1.000</t>
+          <t>woff2</t>
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>md</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="18">
-      <c r="A18" s="3" t="inlineStr">
-        <is>
-          <t>Original Version</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>exe</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>2019.1.000</t>
+          <t>otf</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>Gemfile</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t>Deployed Revision</t>
-        </is>
-      </c>
-      <c r="B21" s="4" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>lock</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
+          <t>xlsx</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>Deployed Version</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>2019.1.000</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26"/>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>Original Version</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="inlineStr">
+        <is>
+          <t>2019.1.000</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29"/>
+    <row r="30">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>Deployed Revision</t>
+        </is>
+      </c>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="inlineStr">
+        <is>
           <t>rev 20181201</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="inlineStr">
+      <c r="B31" s="5" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n">
+      <c r="B32" s="5" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="24"/>
-    <row r="25">
-      <c r="A25" s="3" t="inlineStr">
+    <row r="33"/>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr">
         <is>
           <t>Original Revision</t>
         </is>
       </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="B34" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="5" t="inlineStr">
+    <row r="35">
+      <c r="A35" s="5" t="inlineStr">
         <is>
           <t>rev 20181201</t>
         </is>
       </c>
-      <c r="B26" s="5" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="5" t="inlineStr">
+      <c r="B35" s="5" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="B27" s="5" t="n">
+      <c r="B36" s="5" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create new CSV report which is best viewed in Excel from a Ruby script.
Report is generated from the DocID element of each main schema file and shows a summary of it's child elements values.  Re-generate all reports.  Update README.
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -125,9 +125,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$2:$A$22</c:f>
+              <c:f>'Chart Report'!$A$2:$A$23</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>xsd</c:v>
                 </c:pt>
@@ -138,57 +138,60 @@
                   <c:v>folders</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>html</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>js</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>txt</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>html</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>css</c:v>
+                  <c:v>rb</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>png</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>css</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>ttf</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>sh</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>rb</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>woff</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>woff2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>md</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>eot</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>svg</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>woff2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>md</c:v>
-                </c:pt>
                 <c:pt idx="16">
+                  <c:v>csv</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>exe</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>otf</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Gemfile</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>lock</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>xlsx</c:v>
                 </c:pt>
               </c:strCache>
@@ -196,36 +199,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$2:$B$22</c:f>
+              <c:f>'Chart Report'!$B$2:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>230</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>31</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>4</c:v>
@@ -261,6 +264,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -330,9 +336,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$2:$A$22</c:f>
+              <c:f>'Chart Report'!$A$2:$A$23</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>xsd</c:v>
                 </c:pt>
@@ -343,57 +349,60 @@
                   <c:v>folders</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>html</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>js</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>txt</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>html</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>css</c:v>
+                  <c:v>rb</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>png</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>css</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>ttf</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>sh</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>rb</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>woff</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>woff2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>md</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>eot</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>svg</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>woff2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>md</c:v>
-                </c:pt>
                 <c:pt idx="16">
+                  <c:v>csv</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>exe</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>otf</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Gemfile</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>lock</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>xlsx</c:v>
                 </c:pt>
               </c:strCache>
@@ -401,36 +410,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$2:$B$22</c:f>
+              <c:f>'Chart Report'!$B$2:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>230</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>31</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>4</c:v>
@@ -466,6 +475,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -473,11 +485,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="1182702"/>
-        <c:axId val="8456010"/>
+        <c:axId val="11806951"/>
+        <c:axId val="8468585"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1182702"/>
+        <c:axId val="11806951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -498,7 +510,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8456010"/>
+        <c:crossAx val="8468585"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -507,7 +519,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8456010"/>
+        <c:axId val="8468585"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +540,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1182702"/>
+        <c:crossAx val="11806951"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -593,7 +605,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$25:$A$25</c:f>
+              <c:f>'Chart Report'!$A$26:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -604,12 +616,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$25:$B$25</c:f>
+              <c:f>'Chart Report'!$B$26:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,7 +689,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$28:$A$28</c:f>
+              <c:f>'Chart Report'!$A$29:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -688,12 +700,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$28:$B$28</c:f>
+              <c:f>'Chart Report'!$B$29:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -761,7 +773,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$31:$A$32</c:f>
+              <c:f>'Chart Report'!$A$32:$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -775,12 +787,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$31:$B$32</c:f>
+              <c:f>'Chart Report'!$B$32:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>108</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -851,7 +863,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$35:$A$36</c:f>
+              <c:f>'Chart Report'!$A$36:$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -865,12 +877,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$35:$B$36</c:f>
+              <c:f>'Chart Report'!$B$36:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>108</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -1088,7 +1100,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1117,7 +1129,7 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3">
@@ -1137,23 +1149,23 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>js</t>
+          <t>html</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>txt</t>
+          <t>js</t>
         </is>
       </c>
       <c r="B6" s="5" t="n">
@@ -1163,21 +1175,21 @@
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>html</t>
+          <t>txt</t>
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>css</t>
+          <t>rb</t>
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -1193,17 +1205,17 @@
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>ttf</t>
+          <t>css</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>sh</t>
+          <t>ttf</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
@@ -1213,7 +1225,7 @@
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>rb</t>
+          <t>sh</t>
         </is>
       </c>
       <c r="B12" s="5" t="n">
@@ -1233,7 +1245,7 @@
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>eot</t>
+          <t>woff2</t>
         </is>
       </c>
       <c r="B14" s="5" t="n">
@@ -1243,7 +1255,7 @@
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>svg</t>
+          <t>md</t>
         </is>
       </c>
       <c r="B15" s="5" t="n">
@@ -1253,7 +1265,7 @@
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>woff2</t>
+          <t>eot</t>
         </is>
       </c>
       <c r="B16" s="5" t="n">
@@ -1263,7 +1275,7 @@
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>md</t>
+          <t>svg</t>
         </is>
       </c>
       <c r="B17" s="5" t="n">
@@ -1273,7 +1285,7 @@
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>exe</t>
+          <t>csv</t>
         </is>
       </c>
       <c r="B18" s="5" t="n">
@@ -1283,7 +1295,7 @@
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>otf</t>
+          <t>exe</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
@@ -1293,7 +1305,7 @@
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>Gemfile</t>
+          <t>otf</t>
         </is>
       </c>
       <c r="B20" s="5" t="n">
@@ -1303,7 +1315,7 @@
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>lock</t>
+          <t>Gemfile</t>
         </is>
       </c>
       <c r="B21" s="5" t="n">
@@ -1313,122 +1325,132 @@
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>xlsx</t>
+          <t>lock</t>
         </is>
       </c>
       <c r="B22" s="5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23"/>
-    <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>xlsx</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>Deployed Version</t>
         </is>
       </c>
-      <c r="B24" s="4" t="inlineStr">
+      <c r="B25" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="5" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
         <is>
           <t>2019.1.000</t>
         </is>
       </c>
-      <c r="B25" s="5" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26"/>
-    <row r="27">
-      <c r="A27" s="3" t="inlineStr">
+      <c r="B26" s="5" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27"/>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
         <is>
           <t>Original Version</t>
         </is>
       </c>
-      <c r="B27" s="4" t="inlineStr">
+      <c r="B28" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="5" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>2019.1.000</t>
         </is>
       </c>
-      <c r="B28" s="5" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29"/>
-    <row r="30">
-      <c r="A30" s="3" t="inlineStr">
+      <c r="B29" s="5" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30"/>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
         <is>
           <t>Deployed Revision</t>
         </is>
       </c>
-      <c r="B30" s="4" t="inlineStr">
+      <c r="B31" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="5" t="inlineStr">
-        <is>
-          <t>rev 20181201</t>
-        </is>
-      </c>
-      <c r="B31" s="5" t="n">
-        <v>108</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="inlineStr">
         <is>
+          <t>rev 20181201</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="B32" s="5" t="n">
+      <c r="B33" s="5" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="33"/>
-    <row r="34">
-      <c r="A34" s="3" t="inlineStr">
+    <row r="34"/>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
         <is>
           <t>Original Revision</t>
         </is>
       </c>
-      <c r="B34" s="4" t="inlineStr">
+      <c r="B35" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="5" t="inlineStr">
-        <is>
-          <t>rev 20181201</t>
-        </is>
-      </c>
-      <c r="B35" s="5" t="n">
-        <v>108</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="inlineStr">
         <is>
+          <t>rev 20181201</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="inlineStr">
+        <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="B36" s="5" t="n">
+      <c r="B37" s="5" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Re-generate charts and update README
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -125,9 +125,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$2:$A$23</c:f>
+              <c:f>'Chart Report'!$A$2:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>xsd</c:v>
                 </c:pt>
@@ -171,49 +171,55 @@
                   <c:v>md</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>svg</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>eot</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>svg</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>csv</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>bat</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>exe</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>otf</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Gemfile</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>lock</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>xlsx</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>xml</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$2:$B$23</c:f>
+              <c:f>'Chart Report'!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>244</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>35</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>10</c:v>
@@ -222,7 +228,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>5</c:v>
@@ -267,6 +273,12 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -336,9 +348,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$2:$A$23</c:f>
+              <c:f>'Chart Report'!$A$2:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>xsd</c:v>
                 </c:pt>
@@ -382,49 +394,55 @@
                   <c:v>md</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>svg</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>eot</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>svg</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>csv</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>bat</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>exe</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>otf</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Gemfile</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>lock</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>xlsx</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>xml</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$2:$B$23</c:f>
+              <c:f>'Chart Report'!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>244</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>35</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>10</c:v>
@@ -433,7 +451,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>5</c:v>
@@ -478,6 +496,12 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -485,11 +509,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="11806951"/>
-        <c:axId val="8468585"/>
+        <c:axId val="5086744"/>
+        <c:axId val="3492548"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="11806951"/>
+        <c:axId val="5086744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +534,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8468585"/>
+        <c:crossAx val="3492548"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -519,7 +543,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8468585"/>
+        <c:axId val="3492548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -540,7 +564,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11806951"/>
+        <c:crossAx val="5086744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -605,7 +629,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$26:$A$26</c:f>
+              <c:f>'Chart Report'!$A$28:$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -616,12 +640,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$26:$B$26</c:f>
+              <c:f>'Chart Report'!$B$28:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>122</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -689,7 +713,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$29:$A$29</c:f>
+              <c:f>'Chart Report'!$A$31:$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -700,12 +724,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$29:$B$29</c:f>
+              <c:f>'Chart Report'!$B$31:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>122</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -773,7 +797,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$32:$A$33</c:f>
+              <c:f>'Chart Report'!$A$34:$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -787,12 +811,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$32:$B$33</c:f>
+              <c:f>'Chart Report'!$B$34:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>115</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -863,7 +887,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$36:$A$37</c:f>
+              <c:f>'Chart Report'!$A$38:$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -877,12 +901,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$36:$B$37</c:f>
+              <c:f>'Chart Report'!$B$38:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>115</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -1100,7 +1124,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1129,7 +1153,7 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3">
@@ -1149,7 +1173,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
@@ -1159,7 +1183,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -1189,7 +1213,7 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -1265,7 +1289,7 @@
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>eot</t>
+          <t>svg</t>
         </is>
       </c>
       <c r="B16" s="5" t="n">
@@ -1275,7 +1299,7 @@
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>svg</t>
+          <t>eot</t>
         </is>
       </c>
       <c r="B17" s="5" t="n">
@@ -1295,7 +1319,7 @@
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>exe</t>
+          <t>bat</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
@@ -1305,7 +1329,7 @@
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>otf</t>
+          <t>exe</t>
         </is>
       </c>
       <c r="B20" s="5" t="n">
@@ -1315,7 +1339,7 @@
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>Gemfile</t>
+          <t>otf</t>
         </is>
       </c>
       <c r="B21" s="5" t="n">
@@ -1325,7 +1349,7 @@
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>lock</t>
+          <t>Gemfile</t>
         </is>
       </c>
       <c r="B22" s="5" t="n">
@@ -1335,122 +1359,142 @@
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>xlsx</t>
+          <t>lock</t>
         </is>
       </c>
       <c r="B23" s="5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24"/>
+    <row r="24">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>xlsx</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="25">
-      <c r="A25" s="3" t="inlineStr">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>xml</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26"/>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
         <is>
           <t>Deployed Version</t>
         </is>
       </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="5" t="inlineStr">
+    <row r="28">
+      <c r="A28" s="5" t="inlineStr">
         <is>
           <t>2019.1.000</t>
         </is>
       </c>
-      <c r="B26" s="5" t="n">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27"/>
-    <row r="28">
-      <c r="A28" s="3" t="inlineStr">
+      <c r="B28" s="5" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29"/>
+    <row r="30">
+      <c r="A30" s="3" t="inlineStr">
         <is>
           <t>Original Version</t>
         </is>
       </c>
-      <c r="B28" s="4" t="inlineStr">
+      <c r="B30" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="5" t="inlineStr">
+    <row r="31">
+      <c r="A31" s="5" t="inlineStr">
         <is>
           <t>2019.1.000</t>
         </is>
       </c>
-      <c r="B29" s="5" t="n">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30"/>
-    <row r="31">
-      <c r="A31" s="3" t="inlineStr">
+      <c r="B31" s="5" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32"/>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
         <is>
           <t>Deployed Revision</t>
         </is>
       </c>
-      <c r="B31" s="4" t="inlineStr">
+      <c r="B33" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="5" t="inlineStr">
+    <row r="34">
+      <c r="A34" s="5" t="inlineStr">
         <is>
           <t>rev 20181201</t>
         </is>
       </c>
-      <c r="B32" s="5" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="5" t="inlineStr">
+      <c r="B34" s="5" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="B33" s="5" t="n">
+      <c r="B35" s="5" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="34"/>
-    <row r="35">
-      <c r="A35" s="3" t="inlineStr">
+    <row r="36"/>
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
         <is>
           <t>Original Revision</t>
         </is>
       </c>
-      <c r="B35" s="4" t="inlineStr">
+      <c r="B37" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="5" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="5" t="inlineStr">
         <is>
           <t>rev 20181201</t>
         </is>
       </c>
-      <c r="B36" s="5" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="5" t="inlineStr">
+      <c r="B38" s="5" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="B37" s="5" t="n">
+      <c r="B39" s="5" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Ruby script clean up and re-generate reports
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -228,7 +228,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>5</c:v>
@@ -451,7 +451,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>5</c:v>
@@ -509,11 +509,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="5086744"/>
-        <c:axId val="3492548"/>
+        <c:axId val="7362536"/>
+        <c:axId val="3735043"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="5086744"/>
+        <c:axId val="7362536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +534,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3492548"/>
+        <c:crossAx val="3735043"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +543,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3492548"/>
+        <c:axId val="3735043"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +564,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5086744"/>
+        <c:crossAx val="7362536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1213,7 +1213,7 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Create shell script to run all 4 reports at once and re-generate reports
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -141,61 +141,61 @@
                   <c:v>html</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>rb</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>js</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>rb</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>txt</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>png</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>sh</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>css</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>ttf</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>sh</c:v>
-                </c:pt>
                 <c:pt idx="11">
+                  <c:v>md</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>eot</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>svg</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>woff</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>woff2</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>md</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>svg</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>eot</c:v>
-                </c:pt>
                 <c:pt idx="16">
+                  <c:v>exe</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Gemfile</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>lock</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>bat</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>csv</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>bat</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>exe</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
+                  <c:v>xlsx</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>otf</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Gemfile</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>lock</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>xlsx</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>xml</c:v>
@@ -210,7 +210,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>250</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
@@ -219,10 +219,10 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>16</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
                   <c:v>10</c:v>
@@ -237,7 +237,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>4</c:v>
@@ -364,61 +364,61 @@
                   <c:v>html</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>rb</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>js</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>rb</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>txt</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>png</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>sh</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>css</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>ttf</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>sh</c:v>
-                </c:pt>
                 <c:pt idx="11">
+                  <c:v>md</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>eot</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>svg</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>woff</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>woff2</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>md</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>svg</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>eot</c:v>
-                </c:pt>
                 <c:pt idx="16">
+                  <c:v>exe</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Gemfile</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>lock</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>bat</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>csv</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>bat</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>exe</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
+                  <c:v>xlsx</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>otf</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Gemfile</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>lock</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>xlsx</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>xml</c:v>
@@ -433,7 +433,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>250</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
@@ -442,10 +442,10 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>16</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
                   <c:v>10</c:v>
@@ -460,7 +460,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>4</c:v>
@@ -509,11 +509,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="6180218"/>
-        <c:axId val="6649038"/>
+        <c:axId val="14195500"/>
+        <c:axId val="8282250"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="6180218"/>
+        <c:axId val="14195500"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +534,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6649038"/>
+        <c:crossAx val="8282250"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +543,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6649038"/>
+        <c:axId val="8282250"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +564,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6180218"/>
+        <c:crossAx val="14195500"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -645,7 +645,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>125</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,7 +729,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>125</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -816,7 +816,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>118</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -906,7 +906,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>118</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
@@ -1183,23 +1183,23 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>js</t>
+          <t>rb</t>
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>rb</t>
+          <t>txt</t>
         </is>
       </c>
       <c r="B7" s="5" t="n">
@@ -1209,7 +1209,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>txt</t>
+          <t>js</t>
         </is>
       </c>
       <c r="B8" s="5" t="n">
@@ -1229,7 +1229,7 @@
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>css</t>
+          <t>sh</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
@@ -1239,17 +1239,17 @@
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>ttf</t>
+          <t>css</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>sh</t>
+          <t>ttf</t>
         </is>
       </c>
       <c r="B12" s="5" t="n">
@@ -1259,7 +1259,7 @@
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>woff</t>
+          <t>md</t>
         </is>
       </c>
       <c r="B13" s="5" t="n">
@@ -1269,7 +1269,7 @@
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>woff2</t>
+          <t>eot</t>
         </is>
       </c>
       <c r="B14" s="5" t="n">
@@ -1279,7 +1279,7 @@
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>md</t>
+          <t>svg</t>
         </is>
       </c>
       <c r="B15" s="5" t="n">
@@ -1289,7 +1289,7 @@
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>svg</t>
+          <t>woff</t>
         </is>
       </c>
       <c r="B16" s="5" t="n">
@@ -1299,7 +1299,7 @@
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>eot</t>
+          <t>woff2</t>
         </is>
       </c>
       <c r="B17" s="5" t="n">
@@ -1309,7 +1309,7 @@
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>csv</t>
+          <t>exe</t>
         </is>
       </c>
       <c r="B18" s="5" t="n">
@@ -1319,7 +1319,7 @@
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>bat</t>
+          <t>Gemfile</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
@@ -1329,7 +1329,7 @@
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>exe</t>
+          <t>lock</t>
         </is>
       </c>
       <c r="B20" s="5" t="n">
@@ -1339,7 +1339,7 @@
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>otf</t>
+          <t>bat</t>
         </is>
       </c>
       <c r="B21" s="5" t="n">
@@ -1349,7 +1349,7 @@
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>Gemfile</t>
+          <t>csv</t>
         </is>
       </c>
       <c r="B22" s="5" t="n">
@@ -1359,7 +1359,7 @@
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>lock</t>
+          <t>xlsx</t>
         </is>
       </c>
       <c r="B23" s="5" t="n">
@@ -1369,7 +1369,7 @@
     <row r="24">
       <c r="A24" s="5" t="inlineStr">
         <is>
-          <t>xlsx</t>
+          <t>otf</t>
         </is>
       </c>
       <c r="B24" s="5" t="n">
@@ -1406,7 +1406,7 @@
         </is>
       </c>
       <c r="B28" s="5" t="n">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29"/>
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32"/>
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35">
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="B38" s="5" t="n">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39">

</xml_diff>

<commit_message>
Update docs and re-generate reports
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -210,7 +210,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>270</c:v>
+                  <c:v>274</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
@@ -433,7 +433,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>270</c:v>
+                  <c:v>274</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
@@ -509,11 +509,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="14195500"/>
-        <c:axId val="8282250"/>
+        <c:axId val="3105939"/>
+        <c:axId val="8272626"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="14195500"/>
+        <c:axId val="3105939"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +534,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8282250"/>
+        <c:crossAx val="8272626"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +543,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8282250"/>
+        <c:axId val="8272626"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +564,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14195500"/>
+        <c:crossAx val="3105939"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -645,7 +645,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>135</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,7 +729,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>135</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -816,7 +816,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>128</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -906,7 +906,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>128</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3">
@@ -1406,7 +1406,7 @@
         </is>
       </c>
       <c r="B28" s="5" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29"/>
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32"/>
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35">
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="B38" s="5" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39">

</xml_diff>

<commit_message>
Add latest schema and regenerate reports
Deploy schema
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -210,7 +210,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>274</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
@@ -219,13 +219,13 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>26</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
                   <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>10</c:v>
@@ -433,7 +433,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>274</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>142</c:v>
@@ -442,13 +442,13 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>26</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
                   <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>10</c:v>
@@ -509,11 +509,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="3105939"/>
-        <c:axId val="8272626"/>
+        <c:axId val="5124278"/>
+        <c:axId val="7237959"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="3105939"/>
+        <c:axId val="5124278"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +534,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8272626"/>
+        <c:crossAx val="7237959"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +543,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8272626"/>
+        <c:axId val="7237959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +564,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3105939"/>
+        <c:crossAx val="5124278"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -645,7 +645,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>137</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,7 +729,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>137</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -816,7 +816,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>130</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -906,7 +906,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>130</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -1406,7 +1406,7 @@
         </is>
       </c>
       <c r="B28" s="5" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29"/>
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32"/>
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35">
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="B38" s="5" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39">

</xml_diff>

<commit_message>
Deploy schema and regenerate reports
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -213,16 +213,16 @@
                   <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>142</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>28</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
                   <c:v>11</c:v>
@@ -436,16 +436,16 @@
                   <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>142</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>28</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
                   <c:v>11</c:v>
@@ -509,11 +509,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="5124278"/>
-        <c:axId val="7237959"/>
+        <c:axId val="6426594"/>
+        <c:axId val="726927"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="5124278"/>
+        <c:axId val="6426594"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +534,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7237959"/>
+        <c:crossAx val="726927"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +543,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7237959"/>
+        <c:axId val="726927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +564,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5124278"/>
+        <c:crossAx val="6426594"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1163,7 +1163,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Fix reports, update Gems.
</commit_message>
<xml_diff>
--- a/tools/output/excel/whole_repository_file_type_count.xlsx
+++ b/tools/output/excel/whole_repository_file_type_count.xlsx
@@ -125,9 +125,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$2:$A$25</c:f>
+              <c:f>'Chart Report'!$A$2:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>xsd</c:v>
                 </c:pt>
@@ -135,10 +135,10 @@
                   <c:v>docx</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>html</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>folders</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>html</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>rb</c:v>
@@ -162,70 +162,73 @@
                   <c:v>ttf</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>md</c:v>
+                  <c:v>woff</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>eot</c:v>
+                  <c:v>py</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>svg</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>woff</c:v>
+                  <c:v>eot</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>woff2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>exe</c:v>
+                  <c:v>xlsx</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Gemfile</c:v>
+                  <c:v>md</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>lock</c:v>
+                  <c:v>otf</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>bat</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>exe</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>lock</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>xml</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Gemfile</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>csv</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>xlsx</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>otf</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>xml</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$2:$B$25</c:f>
+              <c:f>'Chart Report'!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>276</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>33</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>17</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>10</c:v>
@@ -258,10 +261,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
                   <c:v>1</c:v>
@@ -279,6 +282,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -348,9 +354,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$2:$A$25</c:f>
+              <c:f>'Chart Report'!$A$2:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>xsd</c:v>
                 </c:pt>
@@ -358,10 +364,10 @@
                   <c:v>docx</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>html</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>folders</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>html</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>rb</c:v>
@@ -385,70 +391,73 @@
                   <c:v>ttf</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>md</c:v>
+                  <c:v>woff</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>eot</c:v>
+                  <c:v>py</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>svg</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>woff</c:v>
+                  <c:v>eot</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>woff2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>exe</c:v>
+                  <c:v>xlsx</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Gemfile</c:v>
+                  <c:v>md</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>lock</c:v>
+                  <c:v>otf</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>bat</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>exe</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>lock</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>xml</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Gemfile</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>csv</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>xlsx</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>otf</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>xml</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$2:$B$25</c:f>
+              <c:f>'Chart Report'!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>276</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>33</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>17</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>10</c:v>
@@ -481,10 +490,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
                   <c:v>1</c:v>
@@ -502,6 +511,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -509,11 +521,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="6426594"/>
-        <c:axId val="726927"/>
+        <c:axId val="8701737"/>
+        <c:axId val="7347053"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="6426594"/>
+        <c:axId val="8701737"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +546,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="726927"/>
+        <c:crossAx val="7347053"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +555,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="726927"/>
+        <c:axId val="7347053"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +576,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6426594"/>
+        <c:crossAx val="8701737"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -629,7 +641,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$28:$A$28</c:f>
+              <c:f>'Chart Report'!$A$29:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -640,12 +652,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$28:$B$28</c:f>
+              <c:f>'Chart Report'!$B$29:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>138</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -713,23 +725,29 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$31:$A$31</c:f>
+              <c:f>'Chart Report'!$A$32:$A$33</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2019.1.000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2018.0.001</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$31:$B$31</c:f>
+              <c:f>'Chart Report'!$B$32:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,29 +815,35 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$34:$A$35</c:f>
+              <c:f>'Chart Report'!$A$36:$A$38</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>rev 20181201</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>rev 20180630</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$34:$B$35</c:f>
+              <c:f>'Chart Report'!$B$36:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -887,29 +911,35 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Chart Report'!$A$38:$A$39</c:f>
+              <c:f>'Chart Report'!$A$41:$A$43</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>rev 20181201</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>rev 20180630</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart Report'!$B$38:$B$39</c:f>
+              <c:f>'Chart Report'!$B$41:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1124,7 +1154,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1153,7 +1183,7 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3">
@@ -1169,21 +1199,21 @@
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>folders</t>
+          <t>html</t>
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>html</t>
+          <t>folders</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -1193,7 +1223,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -1203,7 +1233,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -1259,7 +1289,7 @@
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>md</t>
+          <t>woff</t>
         </is>
       </c>
       <c r="B13" s="5" t="n">
@@ -1269,7 +1299,7 @@
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>eot</t>
+          <t>py</t>
         </is>
       </c>
       <c r="B14" s="5" t="n">
@@ -1289,7 +1319,7 @@
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>woff</t>
+          <t>eot</t>
         </is>
       </c>
       <c r="B16" s="5" t="n">
@@ -1309,27 +1339,27 @@
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>exe</t>
+          <t>xlsx</t>
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>Gemfile</t>
+          <t>md</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>lock</t>
+          <t>otf</t>
         </is>
       </c>
       <c r="B20" s="5" t="n">
@@ -1349,7 +1379,7 @@
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>csv</t>
+          <t>exe</t>
         </is>
       </c>
       <c r="B22" s="5" t="n">
@@ -1359,7 +1389,7 @@
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>xlsx</t>
+          <t>lock</t>
         </is>
       </c>
       <c r="B23" s="5" t="n">
@@ -1369,7 +1399,7 @@
     <row r="24">
       <c r="A24" s="5" t="inlineStr">
         <is>
-          <t>otf</t>
+          <t>xml</t>
         </is>
       </c>
       <c r="B24" s="5" t="n">
@@ -1379,123 +1409,163 @@
     <row r="25">
       <c r="A25" s="5" t="inlineStr">
         <is>
-          <t>xml</t>
+          <t>Gemfile</t>
         </is>
       </c>
       <c r="B25" s="5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="26"/>
-    <row r="27">
-      <c r="A27" s="3" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>csv</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27"/>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
         <is>
           <t>Deployed Version</t>
         </is>
       </c>
-      <c r="B27" s="4" t="inlineStr">
+      <c r="B28" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="5" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>2019.1.000</t>
         </is>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B29" s="5" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30"/>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>Original Version</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="inlineStr">
+        <is>
+          <t>2019.1.000</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="n">
         <v>138</v>
       </c>
     </row>
-    <row r="29"/>
-    <row r="30">
-      <c r="A30" s="3" t="inlineStr">
-        <is>
-          <t>Original Version</t>
-        </is>
-      </c>
-      <c r="B30" s="4" t="inlineStr">
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>2018.0.001</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34"/>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>Deployed Revision</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="5" t="inlineStr">
-        <is>
-          <t>2019.1.000</t>
-        </is>
-      </c>
-      <c r="B31" s="5" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32"/>
-    <row r="33">
-      <c r="A33" s="3" t="inlineStr">
-        <is>
-          <t>Deployed Revision</t>
-        </is>
-      </c>
-      <c r="B33" s="4" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="5" t="inlineStr">
+    <row r="36">
+      <c r="A36" s="5" t="inlineStr">
         <is>
           <t>rev 20181201</t>
         </is>
       </c>
-      <c r="B34" s="5" t="n">
+      <c r="B36" s="5" t="n">
         <v>131</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="5" t="inlineStr">
+    <row r="37">
+      <c r="A37" s="5" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="B35" s="5" t="n">
+      <c r="B37" s="5" t="n">
         <v>7</v>
-      </c>
-    </row>
-    <row r="36"/>
-    <row r="37">
-      <c r="A37" s="3" t="inlineStr">
-        <is>
-          <t>Original Revision</t>
-        </is>
-      </c>
-      <c r="B37" s="4" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="inlineStr">
         <is>
+          <t>rev 20180630</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39"/>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>Original Revision</t>
+        </is>
+      </c>
+      <c r="B40" s="4" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="inlineStr">
+        <is>
           <t>rev 20181201</t>
         </is>
       </c>
-      <c r="B38" s="5" t="n">
+      <c r="B41" s="5" t="n">
         <v>131</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="5" t="inlineStr">
+    <row r="42">
+      <c r="A42" s="5" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
-      <c r="B39" s="5" t="n">
+      <c r="B42" s="5" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="inlineStr">
+        <is>
+          <t>rev 20180630</t>
+        </is>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>